<commit_message>
update xlsx and boards
</commit_message>
<xml_diff>
--- a/Mapki.xlsx
+++ b/Mapki.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oleko\IdeaProjects\PacMan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5300D9B6-814E-4191-93FA-594990D1FECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F44A82A-5ECB-4600-87AF-30D814A2858B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1545" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{91F98ABD-879C-4D12-8C4B-1AB8EFD506CC}"/>
+    <workbookView xWindow="28680" yWindow="9525" windowWidth="29040" windowHeight="16440" xr2:uid="{91F98ABD-879C-4D12-8C4B-1AB8EFD506CC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="Średnia" sheetId="2" r:id="rId2"/>
+    <sheet name="Duża" sheetId="3" r:id="rId1"/>
+    <sheet name="Średnia" sheetId="1" r:id="rId2"/>
+    <sheet name="Mała" sheetId="4" r:id="rId3"/>
+    <sheet name="Sandbox" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Punkt</t>
   </si>
@@ -52,6 +54,9 @@
   </si>
   <si>
     <t>Lewa</t>
+  </si>
+  <si>
+    <t>kwadrat</t>
   </si>
 </sst>
 </file>
@@ -543,1066 +548,2011 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C43A5E1-DDEB-4B75-B72E-6095B65E8E31}">
-  <dimension ref="A1:T17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19D8B02-28EE-4893-BB2C-0403170CBAA1}">
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:16">
+      <c r="A1">
+        <v>19</v>
+      </c>
+      <c r="B1">
+        <v>18</v>
+      </c>
+      <c r="C1">
+        <v>18</v>
+      </c>
+      <c r="D1">
+        <v>18</v>
+      </c>
+      <c r="E1">
+        <v>18</v>
+      </c>
+      <c r="F1">
+        <v>18</v>
+      </c>
+      <c r="G1">
+        <v>18</v>
+      </c>
+      <c r="H1">
+        <v>18</v>
+      </c>
+      <c r="I1">
+        <v>18</v>
+      </c>
+      <c r="J1">
+        <v>18</v>
+      </c>
+      <c r="K1">
+        <v>18</v>
+      </c>
+      <c r="L1">
+        <v>18</v>
+      </c>
+      <c r="M1">
+        <v>18</v>
+      </c>
+      <c r="N1">
+        <v>18</v>
+      </c>
+      <c r="O1">
+        <v>18</v>
+      </c>
+      <c r="P1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>16</v>
+      </c>
+      <c r="G2">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>16</v>
+      </c>
+      <c r="J2">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>16</v>
+      </c>
+      <c r="L2">
+        <v>16</v>
+      </c>
+      <c r="M2">
+        <v>16</v>
+      </c>
+      <c r="N2">
+        <v>16</v>
+      </c>
+      <c r="O2">
+        <v>16</v>
+      </c>
+      <c r="P2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>16</v>
+      </c>
+      <c r="M3">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>16</v>
+      </c>
+      <c r="O3">
+        <v>16</v>
+      </c>
+      <c r="P3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>16</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <v>16</v>
+      </c>
+      <c r="L4">
+        <v>16</v>
+      </c>
+      <c r="M4">
+        <v>16</v>
+      </c>
+      <c r="N4">
+        <v>16</v>
+      </c>
+      <c r="O4">
+        <v>16</v>
+      </c>
+      <c r="P4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>16</v>
+      </c>
+      <c r="J5">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <v>16</v>
+      </c>
+      <c r="L5">
+        <v>16</v>
+      </c>
+      <c r="M5">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <v>16</v>
+      </c>
+      <c r="O5">
+        <v>16</v>
+      </c>
+      <c r="P5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>16</v>
+      </c>
+      <c r="I6">
+        <v>16</v>
+      </c>
+      <c r="J6">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>16</v>
+      </c>
+      <c r="L6">
+        <v>24</v>
+      </c>
+      <c r="M6">
+        <v>24</v>
+      </c>
+      <c r="N6">
+        <v>16</v>
+      </c>
+      <c r="O6">
+        <v>16</v>
+      </c>
+      <c r="P6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>16</v>
+      </c>
+      <c r="H7">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <v>16</v>
+      </c>
+      <c r="K7">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>17</v>
+      </c>
+      <c r="O7">
+        <v>16</v>
+      </c>
+      <c r="P7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>24</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <v>16</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>17</v>
+      </c>
+      <c r="O8">
+        <v>16</v>
+      </c>
+      <c r="P8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>17</v>
+      </c>
+      <c r="F9">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <v>16</v>
+      </c>
+      <c r="I9">
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>16</v>
+      </c>
+      <c r="L9">
+        <v>18</v>
+      </c>
+      <c r="M9">
+        <v>18</v>
+      </c>
+      <c r="N9">
+        <v>16</v>
+      </c>
+      <c r="O9">
+        <v>16</v>
+      </c>
+      <c r="P9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>16</v>
+      </c>
+      <c r="I10">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>16</v>
+      </c>
+      <c r="K10">
+        <v>16</v>
+      </c>
+      <c r="L10">
+        <v>16</v>
+      </c>
+      <c r="M10">
+        <v>16</v>
+      </c>
+      <c r="N10">
+        <v>16</v>
+      </c>
+      <c r="O10">
+        <v>16</v>
+      </c>
+      <c r="P10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>16</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <v>16</v>
+      </c>
+      <c r="K11">
+        <v>16</v>
+      </c>
+      <c r="L11">
+        <v>16</v>
+      </c>
+      <c r="M11">
+        <v>16</v>
+      </c>
+      <c r="N11">
+        <v>16</v>
+      </c>
+      <c r="O11">
+        <v>16</v>
+      </c>
+      <c r="P11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>24</v>
+      </c>
+      <c r="H12">
+        <v>24</v>
+      </c>
+      <c r="I12">
+        <v>16</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <v>16</v>
+      </c>
+      <c r="L12">
+        <v>16</v>
+      </c>
+      <c r="M12">
+        <v>24</v>
+      </c>
+      <c r="N12">
+        <v>24</v>
+      </c>
+      <c r="O12">
+        <v>16</v>
+      </c>
+      <c r="P12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>16</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>17</v>
+      </c>
+      <c r="J13">
+        <v>16</v>
+      </c>
+      <c r="K13">
+        <v>16</v>
+      </c>
+      <c r="L13">
+        <v>20</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>17</v>
+      </c>
+      <c r="P13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>17</v>
+      </c>
+      <c r="J14">
+        <v>16</v>
+      </c>
+      <c r="K14">
+        <v>16</v>
+      </c>
+      <c r="L14">
+        <v>20</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>17</v>
+      </c>
+      <c r="P14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
+      <c r="D15">
+        <v>16</v>
+      </c>
+      <c r="E15">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>16</v>
+      </c>
+      <c r="G15">
+        <v>18</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+      <c r="I15">
+        <v>16</v>
+      </c>
+      <c r="J15">
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>16</v>
+      </c>
+      <c r="L15">
+        <v>16</v>
+      </c>
+      <c r="M15">
+        <v>18</v>
+      </c>
+      <c r="N15">
+        <v>18</v>
+      </c>
+      <c r="O15">
+        <v>16</v>
+      </c>
+      <c r="P15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>24</v>
+      </c>
+      <c r="E16">
+        <v>24</v>
+      </c>
+      <c r="F16">
+        <v>24</v>
+      </c>
+      <c r="G16">
+        <v>24</v>
+      </c>
+      <c r="H16">
+        <v>24</v>
+      </c>
+      <c r="I16">
+        <v>24</v>
+      </c>
+      <c r="J16">
+        <v>24</v>
+      </c>
+      <c r="K16">
+        <v>24</v>
+      </c>
+      <c r="L16">
+        <v>24</v>
+      </c>
+      <c r="M16">
+        <v>24</v>
+      </c>
+      <c r="N16">
+        <v>24</v>
+      </c>
+      <c r="O16">
+        <v>24</v>
+      </c>
+      <c r="P16">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C43A5E1-DDEB-4B75-B72E-6095B65E8E31}">
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:15">
       <c r="A1" s="2">
         <v>19</v>
       </c>
       <c r="B1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="I1">
         <v>26</v>
       </c>
       <c r="J1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="K1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="L1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="M1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="N1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="O1">
-        <v>26</v>
-      </c>
-      <c r="P1">
-        <v>26</v>
-      </c>
-      <c r="Q1">
-        <v>26</v>
-      </c>
-      <c r="R1">
-        <v>26</v>
-      </c>
-      <c r="S1">
-        <v>26</v>
-      </c>
-      <c r="T1">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:15">
       <c r="A2" s="2">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>17</v>
+      </c>
+      <c r="G2">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>17</v>
+      </c>
+      <c r="K2">
+        <v>16</v>
+      </c>
+      <c r="L2">
+        <v>16</v>
+      </c>
+      <c r="M2">
+        <v>16</v>
+      </c>
+      <c r="N2">
+        <v>16</v>
+      </c>
+      <c r="O2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="2">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>17</v>
+      </c>
+      <c r="K3">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>16</v>
+      </c>
+      <c r="M3">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>16</v>
+      </c>
+      <c r="O3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="2">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>17</v>
+      </c>
+      <c r="K4">
+        <v>16</v>
+      </c>
+      <c r="L4">
+        <v>24</v>
+      </c>
+      <c r="M4">
+        <v>24</v>
+      </c>
+      <c r="N4">
+        <v>24</v>
+      </c>
+      <c r="O4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="2">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>17</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
         <v>21</v>
       </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="2">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>16</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>16</v>
+      </c>
+      <c r="L6">
+        <v>22</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="2">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>16</v>
+      </c>
+      <c r="H7">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <v>16</v>
+      </c>
+      <c r="K7">
+        <v>16</v>
+      </c>
+      <c r="L7">
+        <v>16</v>
+      </c>
+      <c r="M7">
+        <v>18</v>
+      </c>
+      <c r="N7">
+        <v>18</v>
+      </c>
+      <c r="O7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="2">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <v>16</v>
+      </c>
+      <c r="K8">
+        <v>16</v>
+      </c>
+      <c r="L8">
+        <v>16</v>
+      </c>
+      <c r="M8">
+        <v>16</v>
+      </c>
+      <c r="N8">
+        <v>16</v>
+      </c>
+      <c r="O8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="2">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <v>16</v>
+      </c>
+      <c r="I9">
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>16</v>
+      </c>
+      <c r="L9">
+        <v>16</v>
+      </c>
+      <c r="M9">
+        <v>16</v>
+      </c>
+      <c r="N9">
+        <v>16</v>
+      </c>
+      <c r="O9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="2">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>16</v>
+      </c>
+      <c r="I10">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <v>16</v>
+      </c>
+      <c r="K10">
+        <v>16</v>
+      </c>
+      <c r="L10">
+        <v>16</v>
+      </c>
+      <c r="M10">
+        <v>16</v>
+      </c>
+      <c r="N10">
+        <v>16</v>
+      </c>
+      <c r="O10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="2">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>16</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <v>16</v>
+      </c>
+      <c r="K11">
+        <v>16</v>
+      </c>
+      <c r="L11">
+        <v>16</v>
+      </c>
+      <c r="M11">
+        <v>16</v>
+      </c>
+      <c r="N11">
+        <v>16</v>
+      </c>
+      <c r="O11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="2">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>16</v>
+      </c>
+      <c r="I12">
+        <v>16</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <v>16</v>
+      </c>
+      <c r="L12">
+        <v>16</v>
+      </c>
+      <c r="M12">
+        <v>16</v>
+      </c>
+      <c r="N12">
+        <v>16</v>
+      </c>
+      <c r="O12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="2">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>16</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>16</v>
+      </c>
+      <c r="G13">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <v>16</v>
+      </c>
+      <c r="I13">
+        <v>16</v>
+      </c>
+      <c r="J13">
+        <v>16</v>
+      </c>
+      <c r="K13">
+        <v>16</v>
+      </c>
+      <c r="L13">
+        <v>16</v>
+      </c>
+      <c r="M13">
+        <v>16</v>
+      </c>
+      <c r="N13">
+        <v>16</v>
+      </c>
+      <c r="O13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="2">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <v>16</v>
+      </c>
+      <c r="H14">
+        <v>16</v>
+      </c>
+      <c r="I14">
+        <v>16</v>
+      </c>
+      <c r="J14">
+        <v>16</v>
+      </c>
+      <c r="K14">
+        <v>16</v>
+      </c>
+      <c r="L14">
+        <v>16</v>
+      </c>
+      <c r="M14">
+        <v>16</v>
+      </c>
+      <c r="N14">
+        <v>16</v>
+      </c>
+      <c r="O14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="2">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>24</v>
+      </c>
+      <c r="E15">
+        <v>24</v>
+      </c>
+      <c r="F15">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>24</v>
+      </c>
+      <c r="H15">
+        <v>24</v>
+      </c>
+      <c r="I15">
+        <v>24</v>
+      </c>
+      <c r="J15">
+        <v>24</v>
+      </c>
+      <c r="K15">
+        <v>24</v>
+      </c>
+      <c r="L15">
+        <v>24</v>
+      </c>
+      <c r="M15">
+        <v>24</v>
+      </c>
+      <c r="N15">
+        <v>24</v>
+      </c>
+      <c r="O15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1DB814E-329B-4F3D-9DF9-29D28BB6AB17}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1">
+        <v>19</v>
+      </c>
+      <c r="B1">
+        <v>18</v>
+      </c>
+      <c r="C1">
+        <v>18</v>
+      </c>
+      <c r="D1">
+        <v>18</v>
+      </c>
+      <c r="E1">
+        <v>18</v>
+      </c>
+      <c r="F1">
+        <v>18</v>
+      </c>
+      <c r="G1">
+        <v>18</v>
+      </c>
+      <c r="H1">
+        <v>18</v>
+      </c>
+      <c r="I1">
+        <v>18</v>
+      </c>
+      <c r="J1">
+        <v>18</v>
+      </c>
+      <c r="K1">
+        <v>18</v>
+      </c>
+      <c r="L1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>17</v>
+      </c>
       <c r="B2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E3">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F3">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G3">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H3">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I3">
         <v>16</v>
       </c>
       <c r="J3">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K3">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="L3">
-        <v>24</v>
-      </c>
-      <c r="M3">
-        <v>16</v>
-      </c>
-      <c r="N3">
-        <v>24</v>
-      </c>
-      <c r="O3">
-        <v>24</v>
-      </c>
-      <c r="P3">
-        <v>24</v>
-      </c>
-      <c r="Q3">
-        <v>24</v>
-      </c>
-      <c r="R3">
-        <v>24</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>16</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I4">
         <v>16</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>16</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>16</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>16</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E5">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F5">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I5">
         <v>16</v>
       </c>
       <c r="J5">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L5">
-        <v>18</v>
-      </c>
-      <c r="M5">
-        <v>20</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>24</v>
-      </c>
-      <c r="P5">
-        <v>18</v>
-      </c>
-      <c r="Q5">
-        <v>22</v>
-      </c>
-      <c r="R5">
-        <v>16</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>16</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I6">
         <v>16</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L6">
-        <v>16</v>
-      </c>
-      <c r="M6">
-        <v>20</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>17</v>
-      </c>
-      <c r="Q6">
-        <v>20</v>
-      </c>
-      <c r="R6">
-        <v>16</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>16</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H7">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I7">
         <v>16</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K7">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7">
-        <v>16</v>
-      </c>
-      <c r="M7">
-        <v>20</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>17</v>
-      </c>
-      <c r="Q7">
-        <v>20</v>
-      </c>
-      <c r="R7">
-        <v>16</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>16</v>
       </c>
       <c r="D8">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E8">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F8">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G8">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H8">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I8">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J8">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K8">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="L8">
-        <v>24</v>
-      </c>
-      <c r="M8">
-        <v>28</v>
-      </c>
-      <c r="N8">
-        <v>24</v>
-      </c>
-      <c r="O8">
-        <v>24</v>
-      </c>
-      <c r="P8">
-        <v>24</v>
-      </c>
-      <c r="Q8">
-        <v>24</v>
-      </c>
-      <c r="R8">
-        <v>16</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>16</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>16</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>17</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>16</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E10">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F10">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G10">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H10">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I10">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K10">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="L10">
-        <v>24</v>
-      </c>
-      <c r="M10">
-        <v>24</v>
-      </c>
-      <c r="N10">
-        <v>24</v>
-      </c>
-      <c r="O10">
-        <v>24</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>16</v>
-      </c>
-      <c r="R10">
-        <v>16</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>17</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>16</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E11">
         <v>16</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>16</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>16</v>
-      </c>
-      <c r="R11">
-        <v>16</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="2">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>25</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E12">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G12">
         <v>24</v>
       </c>
       <c r="H12">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I12">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="K12">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L12">
-        <v>18</v>
-      </c>
-      <c r="M12">
-        <v>22</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>16</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>16</v>
-      </c>
-      <c r="R12">
-        <v>16</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="2">
-        <v>21</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>16</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>16</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>17</v>
-      </c>
-      <c r="I13">
-        <v>20</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>17</v>
-      </c>
-      <c r="L13">
-        <v>20</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>16</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>16</v>
-      </c>
-      <c r="R13">
-        <v>16</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="2">
-        <v>21</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>16</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>24</v>
-      </c>
-      <c r="F14">
-        <v>24</v>
-      </c>
-      <c r="G14">
-        <v>24</v>
-      </c>
-      <c r="H14">
-        <v>24</v>
-      </c>
-      <c r="I14">
-        <v>24</v>
-      </c>
-      <c r="J14">
-        <v>24</v>
-      </c>
-      <c r="K14">
-        <v>24</v>
-      </c>
-      <c r="L14">
-        <v>24</v>
-      </c>
-      <c r="M14">
-        <v>24</v>
-      </c>
-      <c r="N14">
-        <v>24</v>
-      </c>
-      <c r="O14">
-        <v>24</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>16</v>
-      </c>
-      <c r="R14">
-        <v>16</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="2">
-        <v>21</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="2">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>18</v>
-      </c>
-      <c r="C16">
-        <v>18</v>
-      </c>
-      <c r="D16">
-        <v>18</v>
-      </c>
-      <c r="E16">
-        <v>18</v>
-      </c>
-      <c r="F16">
-        <v>18</v>
-      </c>
-      <c r="G16">
-        <v>18</v>
-      </c>
-      <c r="H16">
-        <v>18</v>
-      </c>
-      <c r="I16">
-        <v>18</v>
-      </c>
-      <c r="J16">
-        <v>18</v>
-      </c>
-      <c r="K16">
-        <v>18</v>
-      </c>
-      <c r="L16">
-        <v>18</v>
-      </c>
-      <c r="M16">
-        <v>18</v>
-      </c>
-      <c r="N16">
-        <v>18</v>
-      </c>
-      <c r="O16">
-        <v>18</v>
-      </c>
-      <c r="P16">
-        <v>18</v>
-      </c>
-      <c r="Q16">
-        <v>18</v>
-      </c>
-      <c r="R16">
-        <v>18</v>
-      </c>
-      <c r="S16">
-        <v>18</v>
-      </c>
-      <c r="T16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" s="2">
-        <v>25</v>
-      </c>
-      <c r="B17">
-        <v>24</v>
-      </c>
-      <c r="C17">
-        <v>24</v>
-      </c>
-      <c r="D17">
-        <v>24</v>
-      </c>
-      <c r="E17">
-        <v>24</v>
-      </c>
-      <c r="F17">
-        <v>24</v>
-      </c>
-      <c r="G17">
-        <v>24</v>
-      </c>
-      <c r="H17">
-        <v>24</v>
-      </c>
-      <c r="I17">
-        <v>24</v>
-      </c>
-      <c r="J17">
-        <v>24</v>
-      </c>
-      <c r="K17">
-        <v>24</v>
-      </c>
-      <c r="L17">
-        <v>24</v>
-      </c>
-      <c r="M17">
-        <v>24</v>
-      </c>
-      <c r="N17">
-        <v>24</v>
-      </c>
-      <c r="O17">
-        <v>24</v>
-      </c>
-      <c r="P17">
-        <v>24</v>
-      </c>
-      <c r="Q17">
-        <v>24</v>
-      </c>
-      <c r="R17">
-        <v>24</v>
-      </c>
-      <c r="S17">
-        <v>24</v>
-      </c>
-      <c r="T17">
         <v>28</v>
       </c>
     </row>
@@ -1611,12 +2561,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B6738A-0593-47FF-B550-718D0C4296D8}">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J52" sqref="G49:J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3206,7 +4156,207 @@
         <v>8</v>
       </c>
     </row>
+    <row r="48" spans="3:17">
+      <c r="G48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="7:10">
+      <c r="G49">
+        <v>16</v>
+      </c>
+      <c r="H49">
+        <v>24</v>
+      </c>
+      <c r="I49">
+        <v>24</v>
+      </c>
+      <c r="J49">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10">
+      <c r="G50">
+        <v>20</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="7:10">
+      <c r="G51">
+        <v>20</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="7:10">
+      <c r="G52">
+        <v>16</v>
+      </c>
+      <c r="H52">
+        <v>18</v>
+      </c>
+      <c r="I52">
+        <v>18</v>
+      </c>
+      <c r="J52">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:O12 B13:H13 K13:O13 B14:O15">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThan">
+      <formula>16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:O12 B14:O15 B13:H13 K13:O13">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:Q20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8:K9">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R25 K35 C21:P34">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q21:Q34">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R25 K35 C20:Q34">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{152FDACE-6B02-4FAB-A2E7-0468615ADD16}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R6:V6 B1:O6 B7:H9 L7:O9 B10:O12 R2:V2 I7 I9 B14:O15 B13:H13 K13:O13">
     <cfRule type="colorScale" priority="23">
       <colorScale>
@@ -3291,143 +4441,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K9">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J8">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:O12 B14:O15 B13:H13 K13:O13">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThan">
-      <formula>16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R25 K35 C21:P34">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q21:Q34">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20:Q20">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R25 K35 C20:Q34">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{152FDACE-6B02-4FAB-A2E7-0468615ADD16}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>